<commit_message>
Adding Testcase number 113
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner.xlsx
+++ b/resources/test_data/TestRunner.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22410"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{801244B4-C5BE-4F11-BB03-BE6B380BD87D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B82C8855-3E0E-4291-B84B-19B08F54A83B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -39,13 +39,16 @@
     <t>Smoke</t>
   </si>
   <si>
-    <t>Groups=Smoke</t>
+    <t>Groups=Retesting</t>
   </si>
   <si>
     <t>Regression</t>
   </si>
   <si>
     <t>Sanity</t>
+  </si>
+  <si>
+    <t>Retesting</t>
   </si>
 </sst>
 </file>
@@ -400,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -499,6 +502,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>113</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Waits and pageprocess changes
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner.xlsx
+++ b/resources/test_data/TestRunner.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22410"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B82C8855-3E0E-4291-B84B-19B08F54A83B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC4F843F-5F62-4E7D-874C-85C0E84618EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>Smoke</t>
   </si>
   <si>
-    <t>Groups=Retesting</t>
+    <t>Groups=Smoke</t>
   </si>
   <si>
     <t>Regression</t>

</xml_diff>

<commit_message>
Extent report improvements, NullPointerException bug fix
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner.xlsx
+++ b/resources/test_data/TestRunner.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22410"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F12B9BB-A782-4198-99BC-3E6444DF1839}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D71FE929-8910-4082-8202-08ACE26EE873}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>Smoke</t>
   </si>
   <si>
-    <t>TestCaseNumber=All</t>
+    <t>Groups=Smoke</t>
   </si>
   <si>
     <t>Regression</t>
@@ -403,7 +403,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
latest test data and few changes to the newsubmissions page
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner.xlsx
+++ b/resources/test_data/TestRunner.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22410"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D71FE929-8910-4082-8202-08ACE26EE873}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="TestRunner" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -39,20 +43,20 @@
     <t>Smoke</t>
   </si>
   <si>
-    <t>Groups=Smoke</t>
-  </si>
-  <si>
     <t>Regression</t>
   </si>
   <si>
     <t>Sanity</t>
+  </si>
+  <si>
+    <t>Groups=Smoke,Regression</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,8 +94,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -399,21 +431,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -424,7 +456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>101</v>
       </c>
@@ -432,10 +464,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>102</v>
       </c>
@@ -443,23 +475,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>105</v>
       </c>
@@ -467,36 +499,52 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>110</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>111</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Test case priority functionality
New Priority column in TestRunner.xlsx
Sort by priority functionality implemented

Columns now retrieved dynamically by Heading (top cell)
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner.xlsx
+++ b/resources/test_data/TestRunner.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22413"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{D71FE929-8910-4082-8202-08ACE26EE873}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CBE16BE5-FDA6-47D8-AAF7-F19BBA694AF0}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestRunner" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>TestCaseNumber</t>
   </si>
   <si>
-    <t>Groups</t>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Group</t>
   </si>
   <si>
     <t>Execution</t>
@@ -43,20 +42,20 @@
     <t>Smoke</t>
   </si>
   <si>
+    <t>All</t>
+  </si>
+  <si>
     <t>Regression</t>
   </si>
   <si>
     <t>Sanity</t>
-  </si>
-  <si>
-    <t>Groups=Smoke,Regression</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,43 +86,15 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7D7D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
-    </tableStyle>
-  </tableStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -431,120 +402,156 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" customWidth="1"/>
+    <col min="1" max="2" width="21.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>101</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="B2" s="1">
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>102</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>103</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>104</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>105</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>106</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>107</v>
       </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>108</v>
       </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>109</v>
       </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>110</v>
       </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>111</v>
       </c>
-      <c r="B12" t="s">
-        <v>5</v>
+      <c r="B12" s="1">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ContinueIfException property implemented for NoDev
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner.xlsx
+++ b/resources/test_data/TestRunner.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22413"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{D71FE929-8910-4082-8202-08ACE26EE873}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CBE16BE5-FDA6-47D8-AAF7-F19BBA694AF0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5F85309-2AC2-4CC2-86D0-397D55163BE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
     <t>Smoke</t>
   </si>
   <si>
-    <t>All</t>
+    <t>TestCaseNumber=All</t>
   </si>
   <si>
     <t>Regression</t>
@@ -406,7 +406,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Individual test cases will accept multiple groups separated by comma values in test runner file
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner.xlsx
+++ b/resources/test_data/TestRunner.xlsx
@@ -3,12 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22413"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5F85309-2AC2-4CC2-86D0-397D55163BE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1114\AC\Temp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3836CDCA-7EAE-43C8-9078-6932D3A9A8AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TestRunner" sheetId="1" r:id="rId1"/>
+    <sheet name="Config" sheetId="2" r:id="rId1"/>
+    <sheet name="Test Cases" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -25,7 +31,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+  <si>
+    <t>Properties</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>RunInParallel</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>NumberOfWindows</t>
+  </si>
+  <si>
+    <t>BaseURL</t>
+  </si>
+  <si>
+    <t>https://vam-bd-agentuw-qa-wapp.azurewebsites.net</t>
+  </si>
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -33,19 +66,31 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <t>Execution</t>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>Execute</t>
+  </si>
+  <si>
+    <t>Smoke,Smoke</t>
+  </si>
+  <si>
+    <t>Groups=Smoke,Regression</t>
   </si>
   <si>
     <t>Smoke</t>
   </si>
   <si>
-    <t>TestCaseNumber=All</t>
+    <t>Regression,Sanity</t>
   </si>
   <si>
     <t>Regression</t>
+  </si>
+  <si>
+    <t>Sanity,Regression</t>
+  </si>
+  <si>
+    <t>Sanity,Smoke</t>
   </si>
   <si>
     <t>Sanity</t>
@@ -72,9 +117,49 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -84,9 +169,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -402,11 +498,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23DF2C0-F6AE-4FFC-8C16-6932FC7B9D78}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -418,16 +573,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -438,10 +593,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -452,7 +607,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -463,7 +618,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -474,7 +629,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -485,7 +640,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -496,7 +651,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -507,7 +662,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -518,7 +673,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -529,7 +684,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -540,7 +695,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -551,7 +706,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Report will now display fail if the test case is not found in the excel sheet
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner.xlsx
+++ b/resources/test_data/TestRunner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1114\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3836CDCA-7EAE-43C8-9078-6932D3A9A8AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A5C947C-29E9-4B46-ABBC-B791D44009C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
     <t>Smoke,Smoke</t>
   </si>
   <si>
-    <t>Groups=Smoke,Regression</t>
+    <t>TestCaseNumber=All</t>
   </si>
   <si>
     <t>Smoke</t>
@@ -561,7 +561,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Added test configuration capability to TestRunner.xlsx
Could be optimized by moving call "excelConfig" to @BeforeSuite, but
that may require significant refactoring
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner.xlsx
+++ b/resources/test_data/TestRunner.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1114\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A5C947C-29E9-4B46-ABBC-B791D44009C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{5A5C947C-29E9-4B46-ABBC-B791D44009C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7AC95F6E-E9B7-4D24-AEC2-584E4C260143}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="2" r:id="rId1"/>
@@ -51,7 +51,7 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>NumberOfWindows</t>
+    <t>NumberOfBrowsers</t>
   </si>
   <si>
     <t>BaseURL</t>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23DF2C0-F6AE-4FFC-8C16-6932FC7B9D78}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -560,7 +560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated TestData for Orange Hrm
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner.xlsx
+++ b/resources/test_data/TestRunner.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1114\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{5A5C947C-29E9-4B46-ABBC-B791D44009C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7AC95F6E-E9B7-4D24-AEC2-584E4C260143}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{743597BE-1748-456E-AED2-4A74852811A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Properties</t>
   </si>
@@ -57,7 +57,7 @@
     <t>BaseURL</t>
   </si>
   <si>
-    <t>https://vam-bd-agentuw-qa-wapp.azurewebsites.net</t>
+    <t>http://testingmasters.com/hrm/symfony/web/index.php/auth/login</t>
   </si>
   <si>
     <t>TestCaseNumber</t>
@@ -75,7 +75,7 @@
     <t>Smoke,Smoke</t>
   </si>
   <si>
-    <t>TestCaseNumber=All</t>
+    <t>Groups=Orange</t>
   </si>
   <si>
     <t>Smoke</t>
@@ -94,16 +94,33 @@
   </si>
   <si>
     <t>Sanity</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Orange</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -166,8 +183,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -182,11 +200,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -501,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23DF2C0-F6AE-4FFC-8C16-6932FC7B9D78}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -552,16 +571,19 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{78780C9E-BD71-4E1D-9482-59A10EA5F8D4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -709,6 +731,17 @@
         <v>20</v>
       </c>
     </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed bug #95 where URL was not being read properly from Excel
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner.xlsx
+++ b/resources/test_data/TestRunner.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22421"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1114\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{5A5C947C-29E9-4B46-ABBC-B791D44009C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7AC95F6E-E9B7-4D24-AEC2-584E4C260143}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5FF3C75-BCE1-4E39-8C31-0D58D68CF78B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Properties</t>
   </si>
@@ -72,13 +72,10 @@
     <t>Execute</t>
   </si>
   <si>
-    <t>Smoke,Smoke</t>
+    <t>Smoke</t>
   </si>
   <si>
     <t>TestCaseNumber=All</t>
-  </si>
-  <si>
-    <t>Smoke</t>
   </si>
   <si>
     <t>Regression,Sanity</t>
@@ -100,10 +97,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -166,8 +171,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -182,11 +188,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -501,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23DF2C0-F6AE-4FFC-8C16-6932FC7B9D78}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -540,7 +547,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -552,6 +559,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{7049ADED-0D3A-454D-BD53-99493F9E6367}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -560,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -607,7 +617,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -618,7 +628,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -629,7 +639,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -640,7 +650,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -651,7 +661,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -662,7 +672,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -673,7 +683,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -684,7 +694,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -695,7 +705,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -706,7 +716,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update from Xpath to Locators
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner.xlsx
+++ b/resources/test_data/TestRunner.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1114\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5FF3C75-BCE1-4E39-8C31-0D58D68CF78B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="113_{45B379C6-7DBD-471A-BE11-E3E597B4548F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C5FE20CB-DD2F-4269-AE6D-08667BB36F2C}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Config" sheetId="2" r:id="rId1"/>
     <sheet name="Test Cases" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Properties</t>
   </si>
@@ -48,9 +48,6 @@
     <t>RunInParallel</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>NumberOfBrowsers</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>Smoke</t>
   </si>
   <si>
-    <t>TestCaseNumber=All</t>
-  </si>
-  <si>
     <t>Regression,Sanity</t>
   </si>
   <si>
@@ -91,13 +85,19 @@
   </si>
   <si>
     <t>Sanity</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>TestCaseNumber=101</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -509,16 +509,16 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="20.84765625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="53.40234375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -526,7 +526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -534,28 +534,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -571,31 +571,31 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="21.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="1" max="2" width="21.7890625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.9453125" customWidth="1"/>
+    <col min="4" max="4" width="37.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>101</v>
       </c>
@@ -603,13 +603,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>102</v>
       </c>
@@ -617,10 +617,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>103</v>
       </c>
@@ -628,10 +628,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>104</v>
       </c>
@@ -639,10 +639,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>105</v>
       </c>
@@ -650,10 +650,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>106</v>
       </c>
@@ -661,10 +661,10 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>107</v>
       </c>
@@ -672,10 +672,10 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>108</v>
       </c>
@@ -683,10 +683,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>109</v>
       </c>
@@ -694,10 +694,10 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>110</v>
       </c>
@@ -705,10 +705,10 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>111</v>
       </c>
@@ -716,7 +716,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes for bugs #98 and #101
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner.xlsx
+++ b/resources/test_data/TestRunner.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1114\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="113_{45B379C6-7DBD-471A-BE11-E3E597B4548F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C5FE20CB-DD2F-4269-AE6D-08667BB36F2C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{83F5CEC4-804E-482B-BE61-E3C9BACBFEE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="2" r:id="rId1"/>
     <sheet name="Test Cases" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Properties</t>
   </si>
@@ -48,6 +48,9 @@
     <t>RunInParallel</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>NumberOfBrowsers</t>
   </si>
   <si>
@@ -72,6 +75,9 @@
     <t>Smoke</t>
   </si>
   <si>
+    <t>Groups=Regression</t>
+  </si>
+  <si>
     <t>Regression,Sanity</t>
   </si>
   <si>
@@ -85,19 +91,13 @@
   </si>
   <si>
     <t>Sanity</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>TestCaseNumber=101</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -508,17 +508,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23DF2C0-F6AE-4FFC-8C16-6932FC7B9D78}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.84765625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="53.40234375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -526,7 +526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -534,28 +534,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -570,32 +570,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="21.7890625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.9453125" customWidth="1"/>
-    <col min="4" max="4" width="37.125" customWidth="1"/>
+    <col min="1" max="2" width="21.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>101</v>
       </c>
@@ -603,13 +603,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>102</v>
       </c>
@@ -617,10 +617,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>103</v>
       </c>
@@ -628,10 +628,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>104</v>
       </c>
@@ -639,10 +639,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>105</v>
       </c>
@@ -650,10 +650,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>106</v>
       </c>
@@ -661,10 +661,10 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>107</v>
       </c>
@@ -672,10 +672,10 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>108</v>
       </c>
@@ -683,10 +683,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>109</v>
       </c>
@@ -694,10 +694,10 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>110</v>
       </c>
@@ -705,10 +705,10 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>111</v>
       </c>
@@ -716,7 +716,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merge NC_ScreenRecord to Master
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner.xlsx
+++ b/resources/test_data/TestRunner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1114\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83F5CEC4-804E-482B-BE61-E3C9BACBFEE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{479B3CB0-183D-491F-9410-3C8BE19C87CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -509,7 +509,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -571,7 +571,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Merge Code from Master to NoCodeWait
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner.xlsx
+++ b/resources/test_data/TestRunner.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1114\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="113_{45B379C6-7DBD-471A-BE11-E3E597B4548F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C5FE20CB-DD2F-4269-AE6D-08667BB36F2C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{479B3CB0-183D-491F-9410-3C8BE19C87CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="2" r:id="rId1"/>
     <sheet name="Test Cases" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Properties</t>
   </si>
@@ -48,6 +48,9 @@
     <t>RunInParallel</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>NumberOfBrowsers</t>
   </si>
   <si>
@@ -72,6 +75,9 @@
     <t>Smoke</t>
   </si>
   <si>
+    <t>Groups=Regression</t>
+  </si>
+  <si>
     <t>Regression,Sanity</t>
   </si>
   <si>
@@ -85,19 +91,13 @@
   </si>
   <si>
     <t>Sanity</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>TestCaseNumber=101</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -508,17 +508,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23DF2C0-F6AE-4FFC-8C16-6932FC7B9D78}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.84765625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="53.40234375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -526,7 +526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -534,28 +534,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -570,32 +570,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="21.7890625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.9453125" customWidth="1"/>
-    <col min="4" max="4" width="37.125" customWidth="1"/>
+    <col min="1" max="2" width="21.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>101</v>
       </c>
@@ -603,13 +603,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>102</v>
       </c>
@@ -617,10 +617,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>103</v>
       </c>
@@ -628,10 +628,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>104</v>
       </c>
@@ -639,10 +639,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>105</v>
       </c>
@@ -650,10 +650,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>106</v>
       </c>
@@ -661,10 +661,10 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>107</v>
       </c>
@@ -672,10 +672,10 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>108</v>
       </c>
@@ -683,10 +683,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>109</v>
       </c>
@@ -694,10 +694,10 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>110</v>
       </c>
@@ -705,10 +705,10 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>111</v>
       </c>
@@ -716,7 +716,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Task# 105 ReadValue implementation
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner.xlsx
+++ b/resources/test_data/TestRunner.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22505"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1114\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="113_{3707237B-1339-4E6B-BE28-4FEE36772DB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ABBE0FED-845C-40F6-A5AF-C512C03F82F3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{21E45445-A322-41B9-A9E1-B4F5F1D0B531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Config" sheetId="2" r:id="rId1"/>
     <sheet name="Test Cases" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Properties</t>
   </si>
@@ -75,6 +75,9 @@
     <t>Smoke</t>
   </si>
   <si>
+    <t>Groups=Regression</t>
+  </si>
+  <si>
     <t>Regression,Sanity</t>
   </si>
   <si>
@@ -88,16 +91,13 @@
   </si>
   <si>
     <t>Sanity</t>
-  </si>
-  <si>
-    <t>TestCaseNumber=101</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -512,13 +512,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.84765625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="53.40234375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -526,7 +526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -534,7 +534,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -542,7 +542,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -550,7 +550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -571,17 +571,17 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="21.7890625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.9453125" customWidth="1"/>
-    <col min="4" max="4" width="37.125" customWidth="1"/>
+    <col min="1" max="2" width="21.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -595,7 +595,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>101</v>
       </c>
@@ -606,10 +606,10 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>102</v>
       </c>
@@ -620,7 +620,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>103</v>
       </c>
@@ -628,10 +628,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>104</v>
       </c>
@@ -639,10 +639,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>105</v>
       </c>
@@ -650,10 +650,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>106</v>
       </c>
@@ -661,10 +661,10 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>107</v>
       </c>
@@ -672,10 +672,10 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>108</v>
       </c>
@@ -683,10 +683,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>109</v>
       </c>
@@ -694,10 +694,10 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>110</v>
       </c>
@@ -705,10 +705,10 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>111</v>
       </c>
@@ -716,7 +716,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
This task is taking too long to keep locally
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner.xlsx
+++ b/resources/test_data/TestRunner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1114\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21E45445-A322-41B9-A9E1-B4F5F1D0B531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{21E45445-A322-41B9-A9E1-B4F5F1D0B531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{744F31E9-6062-4A36-B763-DDACBD0983E4}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
     <t>Smoke</t>
   </si>
   <si>
-    <t>Groups=Regression</t>
+    <t>TestCaseNumber = 105</t>
   </si>
   <si>
     <t>Regression,Sanity</t>
@@ -571,7 +571,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Update to BizDynamics app
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner.xlsx
+++ b/resources/test_data/TestRunner.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22604"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1114\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F86B75A3-5A1B-48B2-B1A5-12B9BC174F6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{0F03F4EF-DEFF-4B8A-B38A-C81B376313DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5B9D0FBD-A465-4335-9EB8-3925164392C1}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Config" sheetId="2" r:id="rId1"/>
     <sheet name="Test Cases" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Properties</t>
   </si>
@@ -48,7 +48,7 @@
     <t>RunInParallel</t>
   </si>
   <si>
-    <t>Yes</t>
+    <t>No</t>
   </si>
   <si>
     <t>NumberOfBrowsers</t>
@@ -75,7 +75,7 @@
     <t>Smoke</t>
   </si>
   <si>
-    <t>Groups=Smoke</t>
+    <t>TestCaseNumber=101,102,103</t>
   </si>
   <si>
     <t>Regression,Sanity</t>
@@ -91,13 +91,49 @@
   </si>
   <si>
     <t>Sanity</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Description1</t>
+  </si>
+  <si>
+    <t>Description2</t>
+  </si>
+  <si>
+    <t>Description3</t>
+  </si>
+  <si>
+    <t>Description4</t>
+  </si>
+  <si>
+    <t>Description5</t>
+  </si>
+  <si>
+    <t>Description6</t>
+  </si>
+  <si>
+    <t>Description7</t>
+  </si>
+  <si>
+    <t>Description8</t>
+  </si>
+  <si>
+    <t>Description9</t>
+  </si>
+  <si>
+    <t>Description10</t>
+  </si>
+  <si>
+    <t>Description11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +148,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="2">
@@ -509,16 +551,16 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="20.84765625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="53.40234375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -526,7 +568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -534,7 +576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -542,15 +584,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -568,158 +610,195 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="21.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="1" max="3" width="21.7890625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.9453125" customWidth="1"/>
+    <col min="5" max="5" width="37.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>101</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>102</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>103</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>104</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>105</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>106</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1">
         <v>3</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>107</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1">
         <v>3</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>108</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>109</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="1">
         <v>3</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>110</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1">
         <v>4</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>111</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1">
         <v>4</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" alignment="center"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test for failed cases
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner.xlsx
+++ b/resources/test_data/TestRunner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1114\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{0F03F4EF-DEFF-4B8A-B38A-C81B376313DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5B9D0FBD-A465-4335-9EB8-3925164392C1}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{0F03F4EF-DEFF-4B8A-B38A-C81B376313DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{35C10396-80B1-4772-9BBC-4B11C69A9C4D}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Properties</t>
   </si>
@@ -48,9 +48,6 @@
     <t>RunInParallel</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>NumberOfBrowsers</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>Smoke</t>
   </si>
   <si>
-    <t>TestCaseNumber=101,102,103</t>
-  </si>
-  <si>
     <t>Regression,Sanity</t>
   </si>
   <si>
@@ -127,6 +121,30 @@
   </si>
   <si>
     <t>Description11</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>Failed TestCase</t>
+  </si>
+  <si>
+    <t>2222</t>
+  </si>
+  <si>
+    <t>Failed TestCase2</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>TestCaseNumber=1111,2222</t>
   </si>
 </sst>
 </file>
@@ -551,7 +569,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -581,12 +599,12 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
@@ -594,10 +612,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -610,10 +628,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -625,19 +643,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -645,16 +663,16 @@
         <v>101</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -662,13 +680,13 @@
         <v>102</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -676,13 +694,13 @@
         <v>103</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -690,13 +708,13 @@
         <v>104</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -704,13 +722,13 @@
         <v>105</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -718,13 +736,13 @@
         <v>106</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -732,13 +750,13 @@
         <v>107</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -746,13 +764,13 @@
         <v>108</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -760,13 +778,13 @@
         <v>109</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -774,13 +792,13 @@
         <v>110</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -788,13 +806,41 @@
         <v>111</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12" s="1">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>